<commit_message>
Integration of excel file
- Deletion of manual input section
- Replacement with a section that reads the appropriate data from the excel input file
- Minor spelling changes
- Locking of excel cells and sheets to prevent the user from accidentally crashing the code
</commit_message>
<xml_diff>
--- a/stock_input_file.xlsx
+++ b/stock_input_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Coding practice/Python_Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11861023-0E37-124D-BB61-4DB93A136775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364FE42D-D368-674B-B925-C4AEDB4EBAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17080" activeTab="1" xr2:uid="{756C99D0-0F0D-0E4B-B65F-304C87498D43}"/>
+    <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="17080" activeTab="1" xr2:uid="{756C99D0-0F0D-0E4B-B65F-304C87498D43}"/>
   </bookViews>
   <sheets>
     <sheet name="stock_sheet" sheetId="1" r:id="rId1"/>
@@ -76,10 +76,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,19 +88,105 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -108,49 +195,102 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -166,51 +306,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CAFD820B-E5CF-BB4D-8FF2-7BAACB6AE548}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5" xr:uid="{CAFD820B-E5CF-BB4D-8FF2-7BAACB6AE548}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D6772DC-D6D5-EF47-BD40-0FBB8369467D}" name="Table1" displayName="Table1" ref="A1:B1048576" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="5">
+  <autoFilter ref="A1:B1048576" xr:uid="{7D6772DC-D6D5-EF47-BD40-0FBB8369467D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2A6989DF-5521-324C-B7B6-AA5F7B6CB3CB}" name="Stock Ticker" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{129B93BC-8507-CC4A-B0E3-126CA5398704}" name="Amount Invested" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{E4E1FDB9-AF36-3449-99B1-6DD784142C5F}" name="Stock Ticker" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{AD7045D3-5A3E-4540-98B1-ADEEA1A9E625}" name="Amount Invested" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B6D7C18B-6731-3E40-85F7-3261E29451C8}" name="Table2" displayName="Table2" ref="A1:A2" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B6D7C18B-6731-3E40-85F7-3261E29451C8}" name="Table2" displayName="Table2" ref="A1:A2" totalsRowShown="0" headerRowDxfId="14" dataDxfId="0">
   <autoFilter ref="A1:A2" xr:uid="{B6D7C18B-6731-3E40-85F7-3261E29451C8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{673F99A4-2A3A-D342-9B69-CAE54EBCE8AA}" name="Annual Risk Free Rate" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{673F99A4-2A3A-D342-9B69-CAE54EBCE8AA}" name="Annual Risk Free Rate" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}" name="Table4" displayName="Table4" ref="A4:A5" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}" name="Table4" displayName="Table4" ref="A4:A5" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="A4:A5" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FD6CFC6B-AE91-104C-BF41-2FB88AB655AF}" name="Time Interval" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{FD6CFC6B-AE91-104C-BF41-2FB88AB655AF}" name="Time Interval" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}" name="Table5" displayName="Table5" ref="A8:A9" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}" name="Table5" displayName="Table5" ref="A8:A9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="8">
   <autoFilter ref="A8:A9" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{68CB6ED0-AB54-FB44-9379-5355FF31D79F}" name="Start Date" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{68CB6ED0-AB54-FB44-9379-5355FF31D79F}" name="Start Date" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}" name="Table6" displayName="Table6" ref="A11:A12" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}" name="Table6" displayName="Table6" ref="A11:A12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="6">
   <autoFilter ref="A11:A12" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B9AA6F25-A7C2-E146-95F3-F25715C7A69D}" name="End Date" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B9AA6F25-A7C2-E146-95F3-F25715C7A69D}" name="End Date" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -536,56 +676,57 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="12">
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>300</v>
-      </c>
-    </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="11">
         <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>800</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -598,21 +739,21 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="13">
         <v>0.03</v>
       </c>
     </row>
@@ -622,31 +763,32 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>42217</v>
+      <c r="A9" s="6">
+        <v>42186</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>45870</v>
+      <c r="A12" s="6">
+        <v>45839</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5" xr:uid="{53BD9EF3-7DE1-7A47-8605-9EB5BA5DB95E}">
       <formula1>"1d,5d,1wk,1mo,3mo"</formula1>

</xml_diff>

<commit_message>
Modify other parameter input sheet and addition of other parameters sheet in output file
- The parameter sheet in the input excel sheet did not make sense in separated long formats, so the whole sheet was reconfigured to be in one wide table
- Updated the associated code to comply with this change in the input design
- The modification also allowed for a new sheet in the output file to be written, giving the user even more clarity as to what they inputted for an associated output
</commit_message>
<xml_diff>
--- a/stock_input_file.xlsx
+++ b/stock_input_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/Coding practice/Python_Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364FE42D-D368-674B-B925-C4AEDB4EBAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9D7DC9-A82C-BD47-81A4-0183B7B8DC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="17080" activeTab="1" xr2:uid="{756C99D0-0F0D-0E4B-B65F-304C87498D43}"/>
   </bookViews>
@@ -195,9 +195,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -230,11 +229,37 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0000"/>
       <protection locked="0" hidden="0"/>
@@ -242,6 +267,21 @@
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0000"/>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -260,37 +300,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -306,51 +315,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D6772DC-D6D5-EF47-BD40-0FBB8369467D}" name="Table1" displayName="Table1" ref="A1:B1048576" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D6772DC-D6D5-EF47-BD40-0FBB8369467D}" name="Table1" displayName="Table1" ref="A1:B1048576" totalsRowShown="0" dataDxfId="14" tableBorderDxfId="15">
   <autoFilter ref="A1:B1048576" xr:uid="{7D6772DC-D6D5-EF47-BD40-0FBB8369467D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E4E1FDB9-AF36-3449-99B1-6DD784142C5F}" name="Stock Ticker" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{AD7045D3-5A3E-4540-98B1-ADEEA1A9E625}" name="Amount Invested" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E4E1FDB9-AF36-3449-99B1-6DD784142C5F}" name="Stock Ticker" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{AD7045D3-5A3E-4540-98B1-ADEEA1A9E625}" name="Amount Invested" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B6D7C18B-6731-3E40-85F7-3261E29451C8}" name="Table2" displayName="Table2" ref="A1:A2" totalsRowShown="0" headerRowDxfId="14" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B6D7C18B-6731-3E40-85F7-3261E29451C8}" name="Table2" displayName="Table2" ref="A1:A2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="6">
   <autoFilter ref="A1:A2" xr:uid="{B6D7C18B-6731-3E40-85F7-3261E29451C8}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{673F99A4-2A3A-D342-9B69-CAE54EBCE8AA}" name="Annual Risk Free Rate" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{673F99A4-2A3A-D342-9B69-CAE54EBCE8AA}" name="Annual Risk Free Rate" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}" name="Table4" displayName="Table4" ref="A4:A5" totalsRowShown="0" dataDxfId="10">
-  <autoFilter ref="A4:A5" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}" name="Table4" displayName="Table4" ref="B1:B2" totalsRowShown="0" headerRowDxfId="10" dataDxfId="4">
+  <autoFilter ref="B1:B2" xr:uid="{DE643D75-5A06-1D4B-9F12-76170568C61F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FD6CFC6B-AE91-104C-BF41-2FB88AB655AF}" name="Time Interval" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{FD6CFC6B-AE91-104C-BF41-2FB88AB655AF}" name="Time Interval" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}" name="Table5" displayName="Table5" ref="A8:A9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="8">
-  <autoFilter ref="A8:A9" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}" name="Table5" displayName="Table5" ref="C1:C2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="2">
+  <autoFilter ref="C1:C2" xr:uid="{746FEE24-3AC8-F54A-B66E-326D504A5A4D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{68CB6ED0-AB54-FB44-9379-5355FF31D79F}" name="Start Date" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{68CB6ED0-AB54-FB44-9379-5355FF31D79F}" name="Start Date" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}" name="Table6" displayName="Table6" ref="A11:A12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="6">
-  <autoFilter ref="A11:A12" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}" name="Table6" displayName="Table6" ref="D1:D2" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
+  <autoFilter ref="D1:D2" xr:uid="{70BD5DC6-07D1-334F-9425-4D4C92D90C70}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B9AA6F25-A7C2-E146-95F3-F25715C7A69D}" name="End Date" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{B9AA6F25-A7C2-E146-95F3-F25715C7A69D}" name="End Date" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -681,47 +690,47 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>800</v>
       </c>
     </row>
@@ -736,61 +745,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{093AFB86-104B-4B4F-BD1B-AA18AE92005D}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="14" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
+      <c r="B1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+      <c r="C2" s="5">
         <v>42186</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="D2" s="5">
         <v>45839</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5" xr:uid="{53BD9EF3-7DE1-7A47-8605-9EB5BA5DB95E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{53BD9EF3-7DE1-7A47-8605-9EB5BA5DB95E}">
       <formula1>"1d,5d,1wk,1mo,3mo"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>